<commit_message>
Enhance data visualization in data_load_mode.py by adding annotations for initial, exponential, and plateau phases. Adjust y-axis range for better annotation visibility. Update concentration display based on experimental type in summary tables. Include experimental data preview tables for both substrate and enzyme concentration analyses.
</commit_message>
<xml_diff>
--- a/raw/raw_substrate.xlsx
+++ b/raw/raw_substrate.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hyacinth1126\protease-simulator-3\convert_to_csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hyacinth1126\protease-simulator-3\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44710AE8-E387-486B-B6C8-037C186E06B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76366B0-BDE6-40CA-AF7B-56EFFB93E6A9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20820" windowHeight="7845" xr2:uid="{06DE887C-D289-47A0-A687-FB2266CBEDAF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="10">
   <si>
     <t>min</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -431,13 +431,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82AEEC4-7D05-46D8-A69B-2D4965E31F0F}">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1613,6 +1616,1291 @@
         <v>0</v>
       </c>
       <c r="S20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" t="s">
+        <v>6</v>
+      </c>
+      <c r="J22" t="s">
+        <v>6</v>
+      </c>
+      <c r="K22" t="s">
+        <v>7</v>
+      </c>
+      <c r="L22" t="s">
+        <v>7</v>
+      </c>
+      <c r="M22" t="s">
+        <v>7</v>
+      </c>
+      <c r="N22" t="s">
+        <v>8</v>
+      </c>
+      <c r="O22" t="s">
+        <v>8</v>
+      </c>
+      <c r="P22" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>9</v>
+      </c>
+      <c r="R22" t="s">
+        <v>9</v>
+      </c>
+      <c r="S22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>2</v>
+      </c>
+      <c r="J23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K23" t="s">
+        <v>1</v>
+      </c>
+      <c r="L23" t="s">
+        <v>2</v>
+      </c>
+      <c r="M23" t="s">
+        <v>3</v>
+      </c>
+      <c r="N23" t="s">
+        <v>1</v>
+      </c>
+      <c r="O23" t="s">
+        <v>2</v>
+      </c>
+      <c r="P23" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>1</v>
+      </c>
+      <c r="R23" t="s">
+        <v>2</v>
+      </c>
+      <c r="S23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <f>B3-B$3</f>
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <f>E3-E$3</f>
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <f>H3-H$3</f>
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>3</v>
+      </c>
+      <c r="K24">
+        <f>K3-K$3</f>
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>3</v>
+      </c>
+      <c r="N24">
+        <f>N3-N$3</f>
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>3</v>
+      </c>
+      <c r="Q24">
+        <f>Q3-Q$3</f>
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>0.5</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ref="B25:B41" si="0">B4-B$3</f>
+        <v>47939.097970000003</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <f>E4-E$3</f>
+        <v>184907.94931999967</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <f>H4-H$3</f>
+        <v>1465530.5357799996</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>3</v>
+      </c>
+      <c r="K25">
+        <f>K4-K$3</f>
+        <v>869700</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>3</v>
+      </c>
+      <c r="N25">
+        <f>N4-N$3</f>
+        <v>869800</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>3</v>
+      </c>
+      <c r="Q25">
+        <f>Q4-Q$3</f>
+        <v>554800</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>47939.097970000003</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <f t="shared" ref="E25:E41" si="1">E5-E$3</f>
+        <v>184907.94931999967</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+      <c r="H26">
+        <f t="shared" ref="H26:H41" si="2">H5-H$3</f>
+        <v>2568130.5357799996</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>3</v>
+      </c>
+      <c r="K26">
+        <f t="shared" ref="K26:K41" si="3">K5-K$3</f>
+        <v>1102600</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>3</v>
+      </c>
+      <c r="N26">
+        <f t="shared" ref="N26:N41" si="4">N5-N$3</f>
+        <v>1102600</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>3</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" ref="Q26:Q41" si="5">Q5-Q$3</f>
+        <v>691700</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>1.5</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>47939.097970000003</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>-47939.097959999926</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>3</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>3259830.5357799996</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>3</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="3"/>
+        <v>1191600</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>3</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="4"/>
+        <v>1287500</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>3</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="5"/>
+        <v>828700</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="2"/>
+        <v>3444730.5357799996</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>3</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="3"/>
+        <v>1280600</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>3</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="4"/>
+        <v>1424500</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28">
+        <v>3</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="5"/>
+        <v>1150600</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>-89029.753370000049</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="2"/>
+        <v>3533830.5357799996</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>3</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="3"/>
+        <v>1143600</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>3</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="4"/>
+        <v>1650500</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>3</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="5"/>
+        <v>1191700</v>
+      </c>
+      <c r="R29">
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>3.5</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>-47939.097970000003</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>47939.097969999537</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>3</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="2"/>
+        <v>3944730.5357799996</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>3</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="3"/>
+        <v>1328600</v>
+      </c>
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>3</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="4"/>
+        <v>1972400</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30">
+        <v>3</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="5"/>
+        <v>1513600</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>-47939.097970000003</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="2"/>
+        <v>4081630.5357799996</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>3</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="3"/>
+        <v>1102600</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>3</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="4"/>
+        <v>1972400</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>3</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="5"/>
+        <v>1513600</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>-47939.097970000003</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>-273937.7026800001</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>3</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="2"/>
+        <v>4225530.5357799996</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>3</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="3"/>
+        <v>-458900</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>3</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="4"/>
+        <v>2527100</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>3</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="5"/>
+        <v>1513600</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>6.5</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>89029.75337999966</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>3</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="2"/>
+        <v>4362430.5357799996</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>3</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="3"/>
+        <v>1006700</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>3</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="4"/>
+        <v>2253200</v>
+      </c>
+      <c r="O33">
+        <v>0</v>
+      </c>
+      <c r="P33">
+        <v>3</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="5"/>
+        <v>1794300</v>
+      </c>
+      <c r="R33">
+        <v>0</v>
+      </c>
+      <c r="S33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>7</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>-89029.753370000049</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>-47939.097959999926</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>3</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="2"/>
+        <v>4129630.5357799996</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>3</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="3"/>
+        <v>1054600</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>3</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="4"/>
+        <v>2253200</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+      <c r="P34">
+        <v>3</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="5"/>
+        <v>1657400</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>7.5</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>-47939.097970000003</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>47939.097969999537</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>3</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="2"/>
+        <v>4362430.5357799996</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>3</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="3"/>
+        <v>1239500</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>3</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="4"/>
+        <v>2479200</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>3</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="5"/>
+        <v>1972400</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>8</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>95878.195940000005</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>89029.75337999966</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="2"/>
+        <v>4314530.5357799996</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>3</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="3"/>
+        <v>1143600</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>3</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="4"/>
+        <v>2575000</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+      <c r="P36">
+        <v>3</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="5"/>
+        <v>1835400</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="S36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>10</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>-89029.753370000049</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>136968.85135000013</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="2"/>
+        <v>4314530.5357799996</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>3</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="3"/>
+        <v>1328600</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>3</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="4"/>
+        <v>2801000</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>3</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="5"/>
+        <v>2020300</v>
+      </c>
+      <c r="R37">
+        <v>0</v>
+      </c>
+      <c r="S37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>12</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>-47939.097970000003</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>321876.80066000018</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>3</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="2"/>
+        <v>4862430.5357799996</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>3</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="3"/>
+        <v>1143600</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>3</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="4"/>
+        <v>2801000</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+      <c r="P38">
+        <v>3</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="5"/>
+        <v>2068300</v>
+      </c>
+      <c r="R38">
+        <v>0</v>
+      </c>
+      <c r="S38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>14</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>-47939.097970000003</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>89029.75337999966</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>3</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="2"/>
+        <v>4684330.5357799996</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>3</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="3"/>
+        <v>1102600</v>
+      </c>
+      <c r="L39">
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <v>3</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="4"/>
+        <v>2801000</v>
+      </c>
+      <c r="O39">
+        <v>0</v>
+      </c>
+      <c r="P39">
+        <v>3</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="5"/>
+        <v>2253200</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>16</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>95878.195940000005</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>369815.89862999972</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>3</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="2"/>
+        <v>4958230.5357799996</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>3</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="3"/>
+        <v>1883300</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>3</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="4"/>
+        <v>3444800</v>
+      </c>
+      <c r="O40">
+        <v>0</v>
+      </c>
+      <c r="P40">
+        <v>3</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="5"/>
+        <v>2616200</v>
+      </c>
+      <c r="R40">
+        <v>0</v>
+      </c>
+      <c r="S40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>20</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>3</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="1"/>
+        <v>136968.85135000013</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>3</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="2"/>
+        <v>4821330.5357799996</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>3</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="3"/>
+        <v>1602500</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>3</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="4"/>
+        <v>3033900</v>
+      </c>
+      <c r="O41">
+        <v>0</v>
+      </c>
+      <c r="P41">
+        <v>3</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="5"/>
+        <v>2568200</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+      <c r="S41">
         <v>3</v>
       </c>
     </row>

</xml_diff>